<commit_message>
2/1/18, update purchase list stocks
</commit_message>
<xml_diff>
--- a/Modbus_shield_purchase_list.xlsx
+++ b/Modbus_shield_purchase_list.xlsx
@@ -20,7 +20,7 @@
     <sheet name="Web Sheets" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">beth_compile!$A$2:$E$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">beth_compile!$A$2:$E$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">teensy!$A$2:$O$121</definedName>
     <definedName name="en?vendor_0_keywords_PRPC040SACN_RC" localSheetId="5">'Web Sheets'!$A$1:$C$200</definedName>
   </definedNames>
@@ -226,7 +226,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="382">
   <si>
     <t>Part</t>
   </si>
@@ -1329,12 +1329,6 @@
     <t>M2.5x.45 nut</t>
   </si>
   <si>
-    <t>Approx. Order Cost</t>
-  </si>
-  <si>
-    <t>Approx. Cost Per</t>
-  </si>
-  <si>
     <t>Subtotal</t>
   </si>
   <si>
@@ -1375,6 +1369,9 @@
   </si>
   <si>
     <t>485/Power PiHat 2.0 Super Swift</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -1384,7 +1381,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1679,7 +1676,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1742,19 +1739,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1762,7 +1762,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -1781,62 +1781,6 @@
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7044,8 +6988,8 @@
   <dimension ref="A1:O156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K48" sqref="K48"/>
+      <pane ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L63" sqref="L63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7077,14 +7021,14 @@
       <c r="E1" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="55" t="s">
         <v>341</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="53" t="s">
-        <v>380</v>
-      </c>
-      <c r="I1" s="52"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="56" t="s">
+        <v>378</v>
+      </c>
+      <c r="I1" s="55"/>
     </row>
     <row r="2" spans="1:14" s="22" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
@@ -7132,14 +7076,15 @@
         <v>31</v>
       </c>
       <c r="C3" s="39">
-        <v>28.2</v>
+        <f>28.2/3</f>
+        <v>9.4</v>
       </c>
       <c r="D3" s="4">
         <f t="shared" ref="D3:D20" si="0">IF(M3&gt;=(K3-L3),0,J3)</f>
         <v>0</v>
       </c>
       <c r="E3" s="15">
-        <f>D3*C3/3</f>
+        <f>D3*C3</f>
         <v>0</v>
       </c>
       <c r="F3" s="12">
@@ -7172,20 +7117,21 @@
     </row>
     <row r="4" spans="1:14" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="5">
-        <v>28.2</v>
+        <f>28.2/3</f>
+        <v>9.4</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" ref="D4" si="4">IF(M4&gt;=(K4-L4),0,J4)</f>
         <v>0</v>
       </c>
       <c r="E4" s="50">
-        <f>D4*C4/3</f>
+        <f>D4*C4</f>
         <v>0</v>
       </c>
       <c r="F4" s="4">
@@ -7218,21 +7164,22 @@
     </row>
     <row r="5" spans="1:14" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="5">
-        <v>56.4</v>
+        <f>56.4/3</f>
+        <v>18.8</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" ref="D5" si="7">IF(M5&gt;=(K5-L5),0,J5)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E5" s="50">
-        <f>D5*C5/3</f>
-        <v>112.8</v>
+        <f>D5*C5</f>
+        <v>0</v>
       </c>
       <c r="F5" s="4">
         <v>0</v>
@@ -7249,11 +7196,11 @@
         <v>6</v>
       </c>
       <c r="J5" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K5" s="4">
         <f t="shared" ref="K5" si="10">L5+J5</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L5" s="4">
         <v>0</v>
@@ -7274,11 +7221,11 @@
       </c>
       <c r="D6" s="4">
         <f t="shared" ref="D6:D15" si="11">IF(M6&gt;=(K6-L6),0,J6)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E6" s="50">
         <f t="shared" ref="E6:E15" si="12">D6*C6</f>
-        <v>221.94</v>
+        <v>0</v>
       </c>
       <c r="F6" s="4">
         <v>1</v>
@@ -7295,11 +7242,11 @@
         <v>6</v>
       </c>
       <c r="J6" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K6" s="4">
         <f t="shared" ref="K6:K10" si="13">L6+J6</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L6" s="4">
         <v>0</v>
@@ -7315,10 +7262,10 @@
     </row>
     <row r="8" spans="1:14" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C8" s="5">
         <v>1.62</v>
@@ -7352,11 +7299,11 @@
       </c>
       <c r="K8" s="4">
         <f t="shared" si="13"/>
-        <v>0.86</v>
+        <v>0.61</v>
       </c>
       <c r="L8" s="4">
-        <f>86/100</f>
-        <v>0.86</v>
+        <f>61/100</f>
+        <v>0.61</v>
       </c>
       <c r="M8" s="4">
         <v>0</v>
@@ -7364,10 +7311,10 @@
     </row>
     <row r="9" spans="1:14" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C9" s="5">
         <v>2.36</v>
@@ -7401,11 +7348,11 @@
       </c>
       <c r="K9" s="4">
         <f t="shared" si="13"/>
-        <v>0.94</v>
+        <v>0.82</v>
       </c>
       <c r="L9" s="4">
-        <f>94/100</f>
-        <v>0.94</v>
+        <f>82/100</f>
+        <v>0.82</v>
       </c>
       <c r="M9" s="4">
         <v>0</v>
@@ -7413,21 +7360,21 @@
     </row>
     <row r="10" spans="1:14" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C10" s="5">
         <v>0.68</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="14"/>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E10" s="50">
         <f t="shared" si="15"/>
-        <v>16.32</v>
+        <v>0</v>
       </c>
       <c r="F10" s="4">
         <v>4</v>
@@ -7444,11 +7391,11 @@
         <v>24</v>
       </c>
       <c r="J10" s="4">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="K10" s="4">
         <f t="shared" si="13"/>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="L10" s="4">
         <v>0</v>
@@ -7699,11 +7646,11 @@
       </c>
       <c r="D16" s="4">
         <f t="shared" ref="D16" si="23">IF(M16&gt;=(K16-L16),0,J16)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E16" s="15">
         <f>D16*C16</f>
-        <v>87.72</v>
+        <v>0</v>
       </c>
       <c r="F16" s="12">
         <v>1</v>
@@ -7720,11 +7667,11 @@
         <v>6</v>
       </c>
       <c r="J16" s="12">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K16" s="4">
         <f t="shared" ref="K16" si="24">L16+J16</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L16" s="4">
         <v>0</v>
@@ -7815,10 +7762,10 @@
       </c>
       <c r="K20" s="4">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="L20" s="4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="M20" s="4">
         <v>0</v>
@@ -7861,10 +7808,10 @@
       </c>
       <c r="K21" s="4">
         <f t="shared" ref="K21" si="28">L21+J21</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="L21" s="4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="M21" s="4">
         <v>0</v>
@@ -7907,10 +7854,10 @@
       </c>
       <c r="K22" s="4">
         <f t="shared" ref="K22:K23" si="31">L22+J22</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="L22" s="4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="M22" s="4">
         <v>0</v>
@@ -7953,10 +7900,10 @@
       </c>
       <c r="K23" s="4">
         <f t="shared" si="31"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="L23" s="4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="M23" s="4">
         <v>0</v>
@@ -8066,11 +8013,11 @@
       </c>
       <c r="D26" s="4">
         <f t="shared" ref="D26" si="38">IF(M26&gt;=(K26-L26),0,J26)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E26" s="15">
         <f t="shared" ref="E26" si="39">D26*C26</f>
-        <v>19.559999999999999</v>
+        <v>0</v>
       </c>
       <c r="F26" s="12">
         <v>0</v>
@@ -8087,11 +8034,11 @@
         <v>6</v>
       </c>
       <c r="J26" s="12">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K26" s="4">
         <f t="shared" ref="K26" si="42">L26+J26</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L26" s="4">
         <v>0</v>
@@ -8152,10 +8099,10 @@
       </c>
       <c r="K28" s="4">
         <f t="shared" ref="K28:K35" si="46">L28+J28</f>
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="L28" s="4">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="M28" s="4">
         <v>0</v>
@@ -8198,10 +8145,10 @@
       </c>
       <c r="K29" s="4">
         <f t="shared" si="46"/>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="L29" s="4">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="M29" s="4">
         <v>0</v>
@@ -8265,11 +8212,11 @@
       </c>
       <c r="D31" s="4">
         <f t="shared" si="43"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E31" s="15">
         <f>D31*C31</f>
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="F31" s="12">
         <v>3</v>
@@ -8286,14 +8233,14 @@
         <v>18</v>
       </c>
       <c r="J31" s="12">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K31" s="4">
         <f t="shared" si="46"/>
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="L31" s="4">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="M31" s="4">
         <v>0</v>
@@ -8359,11 +8306,11 @@
       </c>
       <c r="D33" s="4">
         <f t="shared" si="43"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E33" s="15">
         <f>D33*C33</f>
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="F33" s="12">
         <v>3</v>
@@ -8380,14 +8327,14 @@
         <v>18</v>
       </c>
       <c r="J33" s="12">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K33" s="4">
         <f t="shared" si="46"/>
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="L33" s="4">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="M33" s="4">
         <v>0</v>
@@ -8406,11 +8353,11 @@
       </c>
       <c r="D34" s="4">
         <f t="shared" si="43"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E34" s="15">
         <f>D34*C34</f>
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="F34" s="12">
         <v>3</v>
@@ -8427,14 +8374,14 @@
         <v>18</v>
       </c>
       <c r="J34" s="12">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K34" s="4">
         <f t="shared" si="46"/>
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="L34" s="4">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="M34" s="4">
         <v>0</v>
@@ -8478,10 +8425,10 @@
       </c>
       <c r="K35" s="4">
         <f t="shared" si="46"/>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="L35" s="4">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="M35" s="4">
         <v>0</v>
@@ -8525,10 +8472,10 @@
       </c>
       <c r="K36" s="4">
         <f t="shared" ref="K36" si="51">L36+J36</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="L36" s="4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="M36" s="4">
         <v>0</v>
@@ -8576,10 +8523,10 @@
       </c>
       <c r="K38" s="4">
         <f>L38+J38</f>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L38" s="4">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="M38" s="4">
         <v>0</v>
@@ -8623,10 +8570,10 @@
       </c>
       <c r="K39" s="4">
         <f>L39+J39</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="L39" s="4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="M39" s="4">
         <v>0</v>
@@ -8670,10 +8617,10 @@
       </c>
       <c r="K40" s="4">
         <f>L40+J40</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="L40" s="4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M40" s="4">
         <v>0</v>
@@ -8720,10 +8667,10 @@
       </c>
       <c r="K42" s="4">
         <f>L42+J42</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="L42" s="4">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="M42" s="4">
         <v>0</v>
@@ -8767,10 +8714,10 @@
       </c>
       <c r="K43" s="4">
         <f>L43+J43</f>
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="L43" s="4">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="M43" s="4">
         <v>0</v>
@@ -8814,10 +8761,10 @@
       </c>
       <c r="K44" s="4">
         <f>L44+J44</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="L44" s="4">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="M44" s="4">
         <v>0</v>
@@ -8928,11 +8875,11 @@
       </c>
       <c r="D48" s="4">
         <f>IF(M48&gt;=(K48-L48),0,J48)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E48" s="15">
         <f>D48*C48</f>
-        <v>6.87</v>
+        <v>0</v>
       </c>
       <c r="F48" s="12">
         <v>1</v>
@@ -8949,14 +8896,14 @@
         <v>6</v>
       </c>
       <c r="J48" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K48" s="4">
         <f>L48+J48</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L48" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M48" s="4">
         <v>0</v>
@@ -8964,7 +8911,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>36</v>
@@ -8999,10 +8946,10 @@
       </c>
       <c r="K49" s="4">
         <f t="shared" si="57"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="L49" s="4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M49" s="4">
         <v>0</v>
@@ -9010,7 +8957,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>36</v>
@@ -9045,10 +8992,10 @@
       </c>
       <c r="K50" s="4">
         <f t="shared" si="57"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="L50" s="4">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="M50" s="4">
         <v>0</v>
@@ -9056,7 +9003,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>36</v>
@@ -9066,11 +9013,11 @@
       </c>
       <c r="D51" s="4">
         <f t="shared" si="53"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E51" s="15">
         <f>D51*C51</f>
-        <v>30.8</v>
+        <v>0</v>
       </c>
       <c r="F51" s="12">
         <v>0</v>
@@ -9087,14 +9034,14 @@
         <v>6</v>
       </c>
       <c r="J51" s="12">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K51" s="4">
         <f t="shared" si="57"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="L51" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M51" s="4">
         <v>0</v>
@@ -9102,7 +9049,7 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>36</v>
@@ -9112,11 +9059,11 @@
       </c>
       <c r="D52" s="4">
         <f t="shared" si="53"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E52" s="15">
         <f>D52*C52</f>
-        <v>42.800000000000004</v>
+        <v>0</v>
       </c>
       <c r="F52" s="12">
         <v>0</v>
@@ -9133,14 +9080,14 @@
         <v>6</v>
       </c>
       <c r="J52" s="12">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K52" s="4">
         <f t="shared" si="57"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L52" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M52" s="4">
         <v>0</v>
@@ -9173,11 +9120,11 @@
       </c>
       <c r="D54" s="4">
         <f>IF(M54&gt;=(K54-L54),0,J54)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E54" s="15">
         <f>D54*C54</f>
-        <v>59.94</v>
+        <v>0</v>
       </c>
       <c r="F54" s="12">
         <v>1</v>
@@ -9194,14 +9141,14 @@
         <v>6</v>
       </c>
       <c r="J54" s="12">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K54" s="4">
         <f>L54+J54</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L54" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M54" s="4">
         <v>0</v>
@@ -9224,7 +9171,7 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>36</v>
@@ -9234,11 +9181,11 @@
       </c>
       <c r="D56" s="4">
         <f>IF(M56&gt;=(K56-L56),0,J56)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E56" s="50">
         <f t="shared" ref="E56" si="58">D56*C56</f>
-        <v>27.42</v>
+        <v>0</v>
       </c>
       <c r="F56" s="4">
         <v>1</v>
@@ -9255,11 +9202,11 @@
         <v>6</v>
       </c>
       <c r="J56" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K56" s="4">
         <f>L56+J56</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="L56" s="4">
         <v>1</v>
@@ -9272,19 +9219,19 @@
       <c r="A57" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C57" s="5">
-        <v>0.16</v>
+        <v>0.22</v>
       </c>
       <c r="D57" s="4">
         <f>IF(M57&gt;=(K57-L57),0,J57)</f>
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E57" s="50">
         <f t="shared" ref="E57:E60" si="61">D57*C57</f>
-        <v>1.6</v>
+        <v>22</v>
       </c>
       <c r="F57" s="4">
         <v>3</v>
@@ -9301,14 +9248,14 @@
         <v>18</v>
       </c>
       <c r="J57" s="4">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="K57" s="4">
         <f>L57+J57</f>
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="L57" s="4">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="M57" s="4">
         <v>0</v>
@@ -9433,11 +9380,11 @@
       </c>
       <c r="D61" s="4">
         <f>IF(M61&gt;=(K61-L61),0,J61)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E61" s="50">
         <f>D61*C61</f>
-        <v>11.100000000000001</v>
+        <v>0</v>
       </c>
       <c r="F61" s="4">
         <v>1</v>
@@ -9454,14 +9401,14 @@
         <v>6</v>
       </c>
       <c r="J61" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K61" s="4">
         <f>L61+J61</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="L61" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M61" s="4">
         <v>0</v>
@@ -9479,11 +9426,11 @@
       </c>
       <c r="D62" s="4">
         <f>IF(M62&gt;=(K62-L62),0,J62)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E62" s="50">
         <f t="shared" ref="E62" si="66">D62*C62</f>
-        <v>19.600000000000001</v>
+        <v>0</v>
       </c>
       <c r="F62" s="4">
         <v>1</v>
@@ -9500,17 +9447,22 @@
         <v>6</v>
       </c>
       <c r="J62" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K62" s="4">
         <f>L62+J62</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="L62" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M62" s="4">
         <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L63" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -10408,17 +10360,17 @@
       </c>
       <c r="E91" s="3">
         <f>SUM(E28:E90)</f>
-        <v>200.58</v>
+        <v>22</v>
       </c>
       <c r="F91" s="3"/>
       <c r="G91" s="2">
         <f>SUMPRODUCT($C$3:$C$90,G3:G90)/$D$1</f>
-        <v>124.29833333333335</v>
+        <v>105.67833333333333</v>
       </c>
       <c r="H91" s="2"/>
       <c r="I91" s="2">
         <f>SUMPRODUCT($C$3:$C$90,I3:I90)/$D$1</f>
-        <v>150.36833333333331</v>
+        <v>112.94833333333331</v>
       </c>
       <c r="J91" t="s">
         <v>70</v>
@@ -10427,12 +10379,12 @@
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I92" s="3">
         <f>SUMPRODUCT($C$3:$C$90,H3:H90)</f>
-        <v>149.81700000000004</v>
+        <v>112.39700000000002</v>
       </c>
       <c r="K92" s="2"/>
       <c r="L92" s="2">
         <f>SUMPRODUCT($C$28:$C$90,L28:L90)</f>
-        <v>79.169999999999987</v>
+        <v>143.77000000000004</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
@@ -10445,24 +10397,24 @@
         <v>40</v>
       </c>
       <c r="E94" s="2">
-        <f>SUMIF($B$3:$B$90,B94,$E$3:$E$90)</f>
-        <v>281.88</v>
+        <f t="shared" ref="E94:E100" si="71">SUMIF($B$3:$B$90,B94,$E$3:$E$90)</f>
+        <v>0</v>
       </c>
       <c r="G94" s="2">
-        <f>SUMPRODUCT(--($B$3:$B$90=$B94),$C$3:$C$90,$G$3:$G$90)/$D$1</f>
+        <f t="shared" ref="G94:G100" si="72">SUMPRODUCT(--($B$3:$B$90=$B94),$C$3:$C$90,$G$3:$G$90)/$D$1</f>
         <v>46.98</v>
       </c>
-      <c r="H94" s="56">
+      <c r="H94" s="52">
         <f>G94/$I$91</f>
-        <v>0.31243280389266359</v>
+        <v>0.41594239253936172</v>
       </c>
       <c r="I94" s="2">
         <f>SUMPRODUCT(--($B$3:$B$90=$B94),$C$3:$C$90,$I$3:$I$90)/$D$1</f>
         <v>46.98</v>
       </c>
-      <c r="J94" s="56">
+      <c r="J94" s="52">
         <f>I94/$I$91</f>
-        <v>0.31243280389266359</v>
+        <v>0.41594239253936172</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.25">
@@ -10470,49 +10422,49 @@
         <v>36</v>
       </c>
       <c r="E95" s="2">
-        <f>SUMIF($B$3:$B$90,B95,$E$3:$E$90)</f>
-        <v>160.19999999999999</v>
+        <f t="shared" si="71"/>
+        <v>22</v>
       </c>
       <c r="G95" s="2">
-        <f>SUMPRODUCT(--($B$3:$B$90=$B95),$C$3:$C$90,$G$3:$G$90)/$D$1</f>
-        <v>22.164999999999996</v>
-      </c>
-      <c r="H95" s="56">
-        <f t="shared" ref="H95:H100" si="71">G95/$I$91</f>
-        <v>0.14740470622138968</v>
+        <f t="shared" si="72"/>
+        <v>22.344999999999999</v>
+      </c>
+      <c r="H95" s="52">
+        <f t="shared" ref="H95:H100" si="73">G95/$I$91</f>
+        <v>0.19783381782230816</v>
       </c>
       <c r="I95" s="2">
-        <f t="shared" ref="I95:I100" si="72">SUMPRODUCT(--($B$3:$B$90=$B95),$C$3:$C$90,$I$3:$I$90)/$D$1</f>
-        <v>28.984999999999999</v>
-      </c>
-      <c r="J95" s="56">
-        <f t="shared" ref="J95:J100" si="73">I95/$I$91</f>
-        <v>0.19276000044335578</v>
+        <f t="shared" ref="I95:I100" si="74">SUMPRODUCT(--($B$3:$B$90=$B95),$C$3:$C$90,$I$3:$I$90)/$D$1</f>
+        <v>29.165000000000003</v>
+      </c>
+      <c r="J95" s="52">
+        <f t="shared" ref="J95:J100" si="75">I95/$I$91</f>
+        <v>0.25821540822499972</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E96" s="2">
-        <f>SUMIF($B$3:$B$90,B96,$E$3:$E$90)</f>
-        <v>16.32</v>
+        <f t="shared" si="71"/>
+        <v>0</v>
       </c>
       <c r="G96" s="2">
-        <f>SUMPRODUCT(--($B$3:$B$90=$B96),$C$3:$C$90,$G$3:$G$90)/$D$1</f>
-        <v>3.3833333333333333</v>
-      </c>
-      <c r="H96" s="56">
-        <f t="shared" si="71"/>
-        <v>2.2500304807084828E-2</v>
-      </c>
-      <c r="I96" s="2">
         <f t="shared" si="72"/>
         <v>3.3833333333333333</v>
       </c>
-      <c r="J96" s="56">
+      <c r="H96" s="52">
         <f t="shared" si="73"/>
-        <v>2.2500304807084828E-2</v>
+        <v>2.9954699051188603E-2</v>
+      </c>
+      <c r="I96" s="2">
+        <f t="shared" si="74"/>
+        <v>3.3833333333333333</v>
+      </c>
+      <c r="J96" s="52">
+        <f t="shared" si="75"/>
+        <v>2.9954699051188603E-2</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
@@ -10520,24 +10472,24 @@
         <v>338</v>
       </c>
       <c r="E97" s="2">
-        <f>SUMIF($B$3:$B$90,B97,$E$3:$E$90)</f>
-        <v>87.72</v>
+        <f t="shared" si="71"/>
+        <v>0</v>
       </c>
       <c r="G97" s="2">
-        <f>SUMPRODUCT(--($B$3:$B$90=$B97),$C$3:$C$90,$G$3:$G$90)/$D$1</f>
-        <v>14.62</v>
-      </c>
-      <c r="H97" s="56">
-        <f t="shared" si="71"/>
-        <v>9.7227918112191183E-2</v>
-      </c>
-      <c r="I97" s="2">
         <f t="shared" si="72"/>
         <v>14.62</v>
       </c>
-      <c r="J97" s="56">
+      <c r="H97" s="52">
         <f t="shared" si="73"/>
-        <v>9.7227918112191183E-2</v>
+        <v>0.12943971432365833</v>
+      </c>
+      <c r="I97" s="2">
+        <f t="shared" si="74"/>
+        <v>14.62</v>
+      </c>
+      <c r="J97" s="52">
+        <f t="shared" si="75"/>
+        <v>0.12943971432365833</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
@@ -10545,23 +10497,23 @@
         <v>39</v>
       </c>
       <c r="E98" s="2">
-        <f>SUMIF($B$3:$B$90,B98,$E$3:$E$90)</f>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="G98" s="2">
-        <f>SUMPRODUCT(--($B$3:$B$90=$B98),$C$3:$C$90,$G$3:$G$90)/$D$1</f>
+        <f t="shared" si="72"/>
         <v>8.9499999999999993</v>
       </c>
-      <c r="H98" s="56">
-        <f t="shared" si="71"/>
-        <v>5.9520510745835233E-2</v>
+      <c r="H98" s="52">
+        <f t="shared" si="73"/>
+        <v>7.9239770396493978E-2</v>
       </c>
       <c r="I98" s="2">
-        <f t="shared" si="72"/>
-        <v>0</v>
-      </c>
-      <c r="J98" s="56">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
+        <v>0</v>
+      </c>
+      <c r="J98" s="52">
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
     </row>
@@ -10570,24 +10522,24 @@
         <v>31</v>
       </c>
       <c r="E99" s="2">
-        <f>SUMIF($B$3:$B$90,B99,$E$3:$E$90)</f>
-        <v>112.8</v>
+        <f t="shared" si="71"/>
+        <v>0</v>
       </c>
       <c r="G99" s="2">
-        <f>SUMPRODUCT(--($B$3:$B$90=$B99),$C$3:$C$90,$G$3:$G$90)/$D$1</f>
-        <v>28.2</v>
-      </c>
-      <c r="H99" s="56">
-        <f t="shared" si="71"/>
-        <v>0.18753948637235235</v>
+        <f t="shared" si="72"/>
+        <v>9.4</v>
+      </c>
+      <c r="H99" s="52">
+        <f t="shared" si="73"/>
+        <v>8.3223892930395921E-2</v>
       </c>
       <c r="I99" s="2">
-        <f t="shared" si="72"/>
-        <v>56.4</v>
-      </c>
-      <c r="J99" s="56">
-        <f t="shared" si="73"/>
-        <v>0.3750789727447047</v>
+        <f t="shared" si="74"/>
+        <v>18.8</v>
+      </c>
+      <c r="J99" s="52">
+        <f t="shared" si="75"/>
+        <v>0.16644778586079184</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
@@ -10598,24 +10550,24 @@
       <c r="C100" s="28"/>
       <c r="D100" s="27"/>
       <c r="E100" s="2">
-        <f>SUMIF($B$3:$B$90,B100,$E$3:$E$90)</f>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="F100" s="30"/>
       <c r="G100" s="2">
-        <f>SUMPRODUCT(--($B$3:$B$90=$B100),$C$3:$C$90,$G$3:$G$90)/$D$1</f>
-        <v>0</v>
-      </c>
-      <c r="H100" s="56">
-        <f t="shared" si="71"/>
+        <f t="shared" si="72"/>
+        <v>0</v>
+      </c>
+      <c r="H100" s="52">
+        <f t="shared" si="73"/>
         <v>0</v>
       </c>
       <c r="I100" s="2">
-        <f t="shared" si="72"/>
-        <v>0</v>
-      </c>
-      <c r="J100" s="56">
-        <f t="shared" si="73"/>
+        <f t="shared" si="74"/>
+        <v>0</v>
+      </c>
+      <c r="J100" s="52">
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="K100" s="27"/>
@@ -10680,16 +10632,16 @@
         <v>0.24</v>
       </c>
       <c r="D104" s="4">
-        <f t="shared" ref="D104:D118" si="74">IF(M104&gt;=(K104-L104),0,J104)</f>
+        <f t="shared" ref="D104:D118" si="76">IF(M104&gt;=(K104-L104),0,J104)</f>
         <v>0</v>
       </c>
       <c r="E104" s="15">
-        <f t="shared" ref="E104:E113" si="75">D104*C104</f>
+        <f t="shared" ref="E104:E113" si="77">D104*C104</f>
         <v>0</v>
       </c>
       <c r="F104" s="44"/>
       <c r="G104" s="12">
-        <f t="shared" ref="G104:G118" si="76">ROUNDUP($D$1*0,0)</f>
+        <f t="shared" ref="G104:G118" si="78">ROUNDUP($D$1*0,0)</f>
         <v>0</v>
       </c>
       <c r="H104" s="12"/>
@@ -10698,7 +10650,7 @@
         <v>0</v>
       </c>
       <c r="K104" s="4">
-        <f t="shared" ref="K104:K118" si="77">L104+J104</f>
+        <f t="shared" ref="K104:K118" si="79">L104+J104</f>
         <v>0</v>
       </c>
       <c r="L104" s="4">
@@ -10719,16 +10671,16 @@
         <v>0.51</v>
       </c>
       <c r="D105" s="4">
-        <f t="shared" si="74"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="E105" s="15">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="F105" s="44"/>
       <c r="G105" s="12">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="H105" s="12"/>
@@ -10737,7 +10689,7 @@
         <v>0</v>
       </c>
       <c r="K105" s="4">
-        <f t="shared" si="77"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="L105" s="4">
@@ -10758,16 +10710,16 @@
         <v>11.95</v>
       </c>
       <c r="D106" s="4">
-        <f t="shared" si="74"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="E106" s="15">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="F106" s="44"/>
       <c r="G106" s="12">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="H106" s="12"/>
@@ -10776,7 +10728,7 @@
         <v>0</v>
       </c>
       <c r="K106" s="4">
-        <f t="shared" si="77"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="L106" s="4">
@@ -10797,16 +10749,16 @@
         <v>0.85</v>
       </c>
       <c r="D107" s="4">
-        <f t="shared" si="74"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="E107" s="15">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="F107" s="44"/>
       <c r="G107" s="12">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="H107" s="12"/>
@@ -10815,7 +10767,7 @@
         <v>0</v>
       </c>
       <c r="K107" s="4">
-        <f t="shared" si="77"/>
+        <f t="shared" si="79"/>
         <v>2</v>
       </c>
       <c r="L107" s="4">
@@ -10836,16 +10788,16 @@
         <v>4.95</v>
       </c>
       <c r="D108" s="4">
-        <f t="shared" si="74"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="E108" s="15">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="F108" s="44"/>
       <c r="G108" s="12">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="H108" s="12"/>
@@ -10854,7 +10806,7 @@
         <v>0</v>
       </c>
       <c r="K108" s="4">
-        <f t="shared" si="77"/>
+        <f t="shared" si="79"/>
         <v>2</v>
       </c>
       <c r="L108" s="4">
@@ -10875,16 +10827,16 @@
         <v>1.5</v>
       </c>
       <c r="D109" s="4">
-        <f t="shared" si="74"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="E109" s="15">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="F109" s="44"/>
       <c r="G109" s="12">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="H109" s="12"/>
@@ -10893,7 +10845,7 @@
         <v>0</v>
       </c>
       <c r="K109" s="4">
-        <f t="shared" si="77"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="L109" s="4">
@@ -10914,16 +10866,16 @@
         <v>1.95</v>
       </c>
       <c r="D110" s="4">
-        <f t="shared" si="74"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="E110" s="15">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="F110" s="44"/>
       <c r="G110" s="12">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="H110" s="12"/>
@@ -10932,7 +10884,7 @@
         <v>0</v>
       </c>
       <c r="K110" s="4">
-        <f t="shared" si="77"/>
+        <f t="shared" si="79"/>
         <v>3</v>
       </c>
       <c r="L110" s="4">
@@ -10953,16 +10905,16 @@
         <v>4.95</v>
       </c>
       <c r="D111" s="4">
-        <f t="shared" si="74"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="E111" s="15">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="F111" s="44"/>
       <c r="G111" s="12">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="H111" s="12"/>
@@ -10971,7 +10923,7 @@
         <v>0</v>
       </c>
       <c r="K111" s="4">
-        <f t="shared" si="77"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="L111" s="4">
@@ -10992,16 +10944,16 @@
         <v>7.62</v>
       </c>
       <c r="D112" s="4">
-        <f t="shared" si="74"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="E112" s="15">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="F112" s="44"/>
       <c r="G112" s="12">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="H112" s="12"/>
@@ -11010,11 +10962,11 @@
         <v>0</v>
       </c>
       <c r="K112" s="4">
-        <f t="shared" si="77"/>
-        <v>0</v>
+        <f t="shared" si="79"/>
+        <v>3</v>
       </c>
       <c r="L112" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M112" s="4">
         <v>0</v>
@@ -11031,16 +10983,16 @@
         <v>12.863</v>
       </c>
       <c r="D113" s="4">
-        <f t="shared" si="74"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="E113" s="15">
-        <f t="shared" si="75"/>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="F113" s="44"/>
       <c r="G113" s="12">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="H113" s="12"/>
@@ -11049,7 +11001,7 @@
         <v>0</v>
       </c>
       <c r="K113" s="4">
-        <f t="shared" si="77"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="L113" s="4">
@@ -11070,7 +11022,7 @@
         <v>4.95</v>
       </c>
       <c r="D114" s="4">
-        <f t="shared" si="74"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="E114" s="15">
@@ -11079,7 +11031,7 @@
       </c>
       <c r="F114" s="44"/>
       <c r="G114" s="12">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="H114" s="12"/>
@@ -11088,7 +11040,7 @@
         <v>0</v>
       </c>
       <c r="K114" s="4">
-        <f t="shared" si="77"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="L114" s="4">
@@ -11109,16 +11061,16 @@
         <v>0.89</v>
       </c>
       <c r="D115" s="4">
-        <f t="shared" si="74"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="E115" s="15">
-        <f t="shared" ref="E115" si="78">D115*C115</f>
+        <f t="shared" ref="E115" si="80">D115*C115</f>
         <v>0</v>
       </c>
       <c r="F115" s="44"/>
       <c r="G115" s="12">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="H115" s="12"/>
@@ -11127,7 +11079,7 @@
         <v>0</v>
       </c>
       <c r="K115" s="4">
-        <f t="shared" si="77"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="L115" s="4">
@@ -11148,16 +11100,16 @@
         <v>0.1</v>
       </c>
       <c r="D116" s="4">
-        <f t="shared" si="74"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="E116" s="15">
-        <f t="shared" ref="E116:E125" si="79">D116*C116</f>
+        <f t="shared" ref="E116:E125" si="81">D116*C116</f>
         <v>0</v>
       </c>
       <c r="F116" s="44"/>
       <c r="G116" s="12">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="H116" s="12"/>
@@ -11166,7 +11118,7 @@
         <v>0</v>
       </c>
       <c r="K116" s="4">
-        <f t="shared" si="77"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="L116" s="4">
@@ -11188,16 +11140,16 @@
         <v>0.1</v>
       </c>
       <c r="D117" s="4">
-        <f t="shared" si="74"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="E117" s="15">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="F117" s="44"/>
       <c r="G117" s="12">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="H117" s="12"/>
@@ -11206,7 +11158,7 @@
         <v>0</v>
       </c>
       <c r="K117" s="4">
-        <f t="shared" si="77"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="L117" s="4">
@@ -11227,16 +11179,16 @@
         <v>1.4</v>
       </c>
       <c r="D118" s="4">
-        <f t="shared" si="74"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="E118" s="15">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="F118" s="44"/>
       <c r="G118" s="12">
-        <f t="shared" si="76"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="H118" s="12"/>
@@ -11245,7 +11197,7 @@
         <v>0</v>
       </c>
       <c r="K118" s="4">
-        <f t="shared" si="77"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="L118" s="4">
@@ -11268,11 +11220,11 @@
         <v>5.3176100000000002</v>
       </c>
       <c r="D119" s="4">
-        <f t="shared" ref="D119:D125" si="80">IF(M119&gt;=(K119-L119),0,J119)</f>
+        <f t="shared" ref="D119:D125" si="82">IF(M119&gt;=(K119-L119),0,J119)</f>
         <v>0</v>
       </c>
       <c r="E119" s="15">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="F119" s="44"/>
@@ -11286,7 +11238,7 @@
         <v>0</v>
       </c>
       <c r="K119" s="4">
-        <f t="shared" ref="K119:K127" si="81">L119+J119</f>
+        <f t="shared" ref="K119:K127" si="83">L119+J119</f>
         <v>0</v>
       </c>
       <c r="L119" s="4">
@@ -11308,11 +11260,11 @@
         <v>7.3530000000000006</v>
       </c>
       <c r="D120" s="4">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>0</v>
       </c>
       <c r="E120" s="15">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="F120" s="44"/>
@@ -11326,7 +11278,7 @@
         <v>0</v>
       </c>
       <c r="K120" s="4">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="L120" s="4">
@@ -11348,11 +11300,11 @@
         <v>7.4749999999999988</v>
       </c>
       <c r="D121" s="4">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>3</v>
       </c>
       <c r="E121" s="15">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>22.424999999999997</v>
       </c>
       <c r="F121" s="44"/>
@@ -11366,7 +11318,7 @@
         <v>3</v>
       </c>
       <c r="K121" s="4">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>3</v>
       </c>
       <c r="L121" s="4">
@@ -11387,16 +11339,16 @@
         <v>19.8</v>
       </c>
       <c r="D122" s="4">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>3</v>
       </c>
       <c r="E122" s="15">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>59.400000000000006</v>
       </c>
       <c r="F122" s="44"/>
       <c r="G122" s="12">
-        <f t="shared" ref="G122:G127" si="82">ROUNDUP($D$1*1,0)</f>
+        <f t="shared" ref="G122:G127" si="84">ROUNDUP($D$1*1,0)</f>
         <v>6</v>
       </c>
       <c r="H122" s="12"/>
@@ -11405,7 +11357,7 @@
         <v>3</v>
       </c>
       <c r="K122" s="4">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>3</v>
       </c>
       <c r="L122" s="4">
@@ -11432,16 +11384,16 @@
         <v>6</v>
       </c>
       <c r="D123" s="4">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>3</v>
       </c>
       <c r="E123" s="15">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>18</v>
       </c>
       <c r="F123" s="44"/>
       <c r="G123" s="12">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>6</v>
       </c>
       <c r="H123" s="12"/>
@@ -11450,7 +11402,7 @@
         <v>3</v>
       </c>
       <c r="K123" s="4">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>3</v>
       </c>
       <c r="L123" s="4">
@@ -11471,16 +11423,16 @@
         <v>20.79</v>
       </c>
       <c r="D124" s="4">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>3</v>
       </c>
       <c r="E124" s="15">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>62.37</v>
       </c>
       <c r="F124" s="44"/>
       <c r="G124" s="12">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>6</v>
       </c>
       <c r="H124" s="12"/>
@@ -11489,7 +11441,7 @@
         <v>3</v>
       </c>
       <c r="K124" s="4">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>3</v>
       </c>
       <c r="L124" s="4">
@@ -11510,16 +11462,16 @@
         <v>0.6</v>
       </c>
       <c r="D125" s="4">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>3</v>
       </c>
       <c r="E125" s="15">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>1.7999999999999998</v>
       </c>
       <c r="F125" s="44"/>
       <c r="G125" s="12">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>6</v>
       </c>
       <c r="H125" s="12"/>
@@ -11528,7 +11480,7 @@
         <v>3</v>
       </c>
       <c r="K125" s="4">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>3</v>
       </c>
       <c r="L125" s="4">
@@ -11549,16 +11501,16 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="D126" s="4">
-        <f t="shared" ref="D126:D133" si="83">IF(M126&gt;=(K126-L126),0,J126)</f>
+        <f t="shared" ref="D126:D133" si="85">IF(M126&gt;=(K126-L126),0,J126)</f>
         <v>3</v>
       </c>
       <c r="E126" s="15">
-        <f t="shared" ref="E126:E133" si="84">D126*C126</f>
+        <f t="shared" ref="E126:E133" si="86">D126*C126</f>
         <v>0.84000000000000008</v>
       </c>
       <c r="F126" s="44"/>
       <c r="G126" s="12">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>6</v>
       </c>
       <c r="H126" s="12"/>
@@ -11567,7 +11519,7 @@
         <v>3</v>
       </c>
       <c r="K126" s="4">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>3</v>
       </c>
       <c r="L126" s="4">
@@ -11597,7 +11549,7 @@
       </c>
       <c r="F127" s="44"/>
       <c r="G127" s="12">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>6</v>
       </c>
       <c r="H127" s="12"/>
@@ -11606,7 +11558,7 @@
         <v>3</v>
       </c>
       <c r="K127" s="4">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>3</v>
       </c>
       <c r="L127" s="4">
@@ -11627,7 +11579,7 @@
         <v>0.62</v>
       </c>
       <c r="D128" s="4">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="E128" s="15">
@@ -11645,7 +11597,7 @@
         <v>0</v>
       </c>
       <c r="K128" s="4">
-        <f t="shared" ref="K128:K133" si="85">L128+J128</f>
+        <f t="shared" ref="K128:K133" si="87">L128+J128</f>
         <v>6</v>
       </c>
       <c r="L128" s="4">
@@ -11666,11 +11618,11 @@
         <v>0.65</v>
       </c>
       <c r="D129" s="4">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>3</v>
       </c>
       <c r="E129" s="15">
-        <f t="shared" si="84"/>
+        <f t="shared" si="86"/>
         <v>1.9500000000000002</v>
       </c>
       <c r="F129" s="44"/>
@@ -11684,7 +11636,7 @@
         <v>3</v>
       </c>
       <c r="K129" s="4">
-        <f t="shared" si="85"/>
+        <f t="shared" si="87"/>
         <v>3</v>
       </c>
       <c r="L129" s="4">
@@ -11705,11 +11657,11 @@
         <v>0.7</v>
       </c>
       <c r="D130" s="4">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>6</v>
       </c>
       <c r="E130" s="15">
-        <f t="shared" si="84"/>
+        <f t="shared" si="86"/>
         <v>4.1999999999999993</v>
       </c>
       <c r="F130" s="44"/>
@@ -11723,7 +11675,7 @@
         <v>6</v>
       </c>
       <c r="K130" s="4">
-        <f t="shared" si="85"/>
+        <f t="shared" si="87"/>
         <v>6</v>
       </c>
       <c r="L130" s="4">
@@ -11744,7 +11696,7 @@
         <v>0.98</v>
       </c>
       <c r="D131" s="4">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>12</v>
       </c>
       <c r="E131" s="15">
@@ -11762,7 +11714,7 @@
         <v>12</v>
       </c>
       <c r="K131" s="4">
-        <f t="shared" si="85"/>
+        <f t="shared" si="87"/>
         <v>12</v>
       </c>
       <c r="L131" s="4">
@@ -11783,11 +11735,11 @@
         <v>0.74</v>
       </c>
       <c r="D132" s="4">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="E132" s="15">
-        <f t="shared" si="84"/>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="F132" s="44"/>
@@ -11801,7 +11753,7 @@
         <v>0</v>
       </c>
       <c r="K132" s="4">
-        <f t="shared" si="85"/>
+        <f t="shared" si="87"/>
         <v>21.875</v>
       </c>
       <c r="L132" s="4">
@@ -11823,11 +11775,11 @@
         <v>0.99</v>
       </c>
       <c r="D133" s="4">
-        <f t="shared" si="83"/>
+        <f t="shared" si="85"/>
         <v>1</v>
       </c>
       <c r="E133" s="15">
-        <f t="shared" si="84"/>
+        <f t="shared" si="86"/>
         <v>0.99</v>
       </c>
       <c r="F133" s="44"/>
@@ -11841,7 +11793,7 @@
         <v>1</v>
       </c>
       <c r="K133" s="4">
-        <f t="shared" si="85"/>
+        <f t="shared" si="87"/>
         <v>3.1749999999999998</v>
       </c>
       <c r="L133" s="4">
@@ -11867,16 +11819,16 @@
         <v>0.1</v>
       </c>
       <c r="D134" s="4">
-        <f t="shared" ref="D134:D139" si="86">IF(M134&gt;=(K134-L134),0,J134)</f>
+        <f t="shared" ref="D134:D139" si="88">IF(M134&gt;=(K134-L134),0,J134)</f>
         <v>0</v>
       </c>
       <c r="E134" s="15">
-        <f t="shared" ref="E134:E139" si="87">D134*C134</f>
+        <f t="shared" ref="E134:E139" si="89">D134*C134</f>
         <v>0</v>
       </c>
       <c r="F134" s="44"/>
       <c r="G134" s="12">
-        <f t="shared" ref="G134:G144" si="88">ROUNDUP($D$1*0,0)</f>
+        <f t="shared" ref="G134:G144" si="90">ROUNDUP($D$1*0,0)</f>
         <v>0</v>
       </c>
       <c r="H134" s="12"/>
@@ -11885,7 +11837,7 @@
         <v>0</v>
       </c>
       <c r="K134" s="4">
-        <f t="shared" ref="K134:K139" si="89">L134+J134</f>
+        <f t="shared" ref="K134:K139" si="91">L134+J134</f>
         <v>0</v>
       </c>
       <c r="L134" s="4">
@@ -11906,16 +11858,16 @@
         <v>0.1</v>
       </c>
       <c r="D135" s="4">
-        <f t="shared" si="86"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="E135" s="15">
-        <f t="shared" si="87"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="F135" s="44"/>
       <c r="G135" s="12">
-        <f t="shared" si="88"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="H135" s="12"/>
@@ -11924,7 +11876,7 @@
         <v>0</v>
       </c>
       <c r="K135" s="4">
-        <f t="shared" si="89"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="L135" s="4">
@@ -11948,16 +11900,16 @@
         <v>0.1</v>
       </c>
       <c r="D136" s="4">
-        <f t="shared" si="86"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="E136" s="15">
-        <f t="shared" si="87"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="F136" s="44"/>
       <c r="G136" s="12">
-        <f t="shared" si="88"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="H136" s="12"/>
@@ -11966,7 +11918,7 @@
         <v>0</v>
       </c>
       <c r="K136" s="4">
-        <f t="shared" si="89"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="L136" s="4">
@@ -11990,16 +11942,16 @@
         <v>0.1</v>
       </c>
       <c r="D137" s="4">
-        <f t="shared" si="86"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="E137" s="15">
-        <f t="shared" si="87"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="F137" s="44"/>
       <c r="G137" s="12">
-        <f t="shared" si="88"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="H137" s="12"/>
@@ -12008,7 +11960,7 @@
         <v>0</v>
       </c>
       <c r="K137" s="4">
-        <f t="shared" si="89"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="L137" s="4">
@@ -12032,16 +11984,16 @@
         <v>0.1</v>
       </c>
       <c r="D138" s="4">
-        <f t="shared" si="86"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="E138" s="15">
-        <f t="shared" si="87"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="F138" s="44"/>
       <c r="G138" s="12">
-        <f t="shared" si="88"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="H138" s="12"/>
@@ -12050,7 +12002,7 @@
         <v>0</v>
       </c>
       <c r="K138" s="4">
-        <f t="shared" si="89"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="L138" s="4">
@@ -12074,16 +12026,16 @@
         <v>0.1</v>
       </c>
       <c r="D139" s="4">
-        <f t="shared" si="86"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="E139" s="15">
-        <f t="shared" si="87"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="F139" s="44"/>
       <c r="G139" s="12">
-        <f t="shared" si="88"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="H139" s="12"/>
@@ -12092,7 +12044,7 @@
         <v>0</v>
       </c>
       <c r="K139" s="4">
-        <f t="shared" si="89"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="L139" s="4">
@@ -12116,16 +12068,16 @@
         <v>0.1</v>
       </c>
       <c r="D140" s="4">
-        <f t="shared" ref="D140:D155" si="90">IF(M140&gt;=(K140-L140),0,J140)</f>
+        <f t="shared" ref="D140:D155" si="92">IF(M140&gt;=(K140-L140),0,J140)</f>
         <v>0</v>
       </c>
       <c r="E140" s="15">
-        <f t="shared" ref="E140:E145" si="91">D140*C140</f>
+        <f t="shared" ref="E140:E145" si="93">D140*C140</f>
         <v>0</v>
       </c>
       <c r="F140" s="44"/>
       <c r="G140" s="12">
-        <f t="shared" si="88"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="H140" s="12"/>
@@ -12134,7 +12086,7 @@
         <v>0</v>
       </c>
       <c r="K140" s="4">
-        <f t="shared" ref="K140:K155" si="92">L140+J140</f>
+        <f t="shared" ref="K140:K155" si="94">L140+J140</f>
         <v>0</v>
       </c>
       <c r="L140" s="4">
@@ -12155,16 +12107,16 @@
         <v>0.3</v>
       </c>
       <c r="D141" s="4">
-        <f t="shared" si="90"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="E141" s="15">
-        <f t="shared" si="91"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="F141" s="44"/>
       <c r="G141" s="12">
-        <f t="shared" si="88"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="H141" s="12"/>
@@ -12173,7 +12125,7 @@
         <v>0</v>
       </c>
       <c r="K141" s="4">
-        <f t="shared" si="92"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="L141" s="4">
@@ -12194,16 +12146,16 @@
         <v>0.3</v>
       </c>
       <c r="D142" s="4">
-        <f t="shared" si="90"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="E142" s="15">
-        <f t="shared" si="91"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="F142" s="44"/>
       <c r="G142" s="12">
-        <f t="shared" si="88"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="H142" s="12"/>
@@ -12212,7 +12164,7 @@
         <v>0</v>
       </c>
       <c r="K142" s="4">
-        <f t="shared" si="92"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="L142" s="4">
@@ -12233,16 +12185,16 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="D143" s="4">
-        <f t="shared" si="90"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="E143" s="15">
-        <f t="shared" si="91"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="F143" s="44"/>
       <c r="G143" s="12">
-        <f t="shared" si="88"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="H143" s="12"/>
@@ -12251,7 +12203,7 @@
         <v>0</v>
       </c>
       <c r="K143" s="4">
-        <f t="shared" si="92"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="L143" s="4">
@@ -12272,16 +12224,16 @@
         <v>2.42</v>
       </c>
       <c r="D144" s="4">
-        <f t="shared" si="90"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="E144" s="15">
-        <f t="shared" si="91"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="F144" s="44"/>
       <c r="G144" s="12">
-        <f t="shared" si="88"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="H144" s="12"/>
@@ -12290,7 +12242,7 @@
         <v>0</v>
       </c>
       <c r="K144" s="4">
-        <f t="shared" si="92"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="L144" s="4">
@@ -12312,11 +12264,11 @@
         <v>2.73</v>
       </c>
       <c r="D145" s="4">
-        <f t="shared" si="90"/>
+        <f t="shared" si="92"/>
         <v>6</v>
       </c>
       <c r="E145" s="15">
-        <f t="shared" si="91"/>
+        <f t="shared" si="93"/>
         <v>16.38</v>
       </c>
       <c r="F145" s="44"/>
@@ -12330,7 +12282,7 @@
         <v>6</v>
       </c>
       <c r="K145" s="4">
-        <f t="shared" si="92"/>
+        <f t="shared" si="94"/>
         <v>6</v>
       </c>
       <c r="L145" s="4">
@@ -12351,11 +12303,11 @@
         <v>2.84</v>
       </c>
       <c r="D146" s="4">
-        <f t="shared" si="90"/>
+        <f t="shared" si="92"/>
         <v>3</v>
       </c>
       <c r="E146" s="15">
-        <f t="shared" ref="E146" si="93">D146*C146</f>
+        <f t="shared" ref="E146" si="95">D146*C146</f>
         <v>8.52</v>
       </c>
       <c r="F146" s="44"/>
@@ -12369,7 +12321,7 @@
         <v>3</v>
       </c>
       <c r="K146" s="4">
-        <f t="shared" si="92"/>
+        <f t="shared" si="94"/>
         <v>3</v>
       </c>
       <c r="L146" s="4">
@@ -12390,7 +12342,7 @@
         <v>5.5</v>
       </c>
       <c r="D147" s="4">
-        <f t="shared" si="90"/>
+        <f t="shared" si="92"/>
         <v>3</v>
       </c>
       <c r="E147" s="15">
@@ -12408,7 +12360,7 @@
         <v>3</v>
       </c>
       <c r="K147" s="4">
-        <f t="shared" si="92"/>
+        <f t="shared" si="94"/>
         <v>3</v>
       </c>
       <c r="L147" s="4">
@@ -12429,11 +12381,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="D148" s="4">
-        <f t="shared" si="90"/>
+        <f t="shared" si="92"/>
         <v>3</v>
       </c>
       <c r="E148" s="15">
-        <f t="shared" ref="E148" si="94">D148*C148</f>
+        <f t="shared" ref="E148" si="96">D148*C148</f>
         <v>3.3000000000000003</v>
       </c>
       <c r="F148" s="44"/>
@@ -12447,7 +12399,7 @@
         <v>3</v>
       </c>
       <c r="K148" s="4">
-        <f t="shared" si="92"/>
+        <f t="shared" si="94"/>
         <v>3</v>
       </c>
       <c r="L148" s="4">
@@ -12468,11 +12420,11 @@
         <v>4.5</v>
       </c>
       <c r="D149" s="4">
-        <f t="shared" si="90"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="E149" s="15">
-        <f t="shared" ref="E149:E154" si="95">D149*C149</f>
+        <f t="shared" ref="E149:E154" si="97">D149*C149</f>
         <v>0</v>
       </c>
       <c r="F149" s="44"/>
@@ -12486,7 +12438,7 @@
         <v>0</v>
       </c>
       <c r="K149" s="4">
-        <f t="shared" si="92"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="L149" s="4">
@@ -12507,11 +12459,11 @@
         <v>0.75</v>
       </c>
       <c r="D150" s="4">
-        <f t="shared" si="90"/>
+        <f t="shared" si="92"/>
         <v>6</v>
       </c>
       <c r="E150" s="15">
-        <f t="shared" si="95"/>
+        <f t="shared" si="97"/>
         <v>4.5</v>
       </c>
       <c r="F150" s="44"/>
@@ -12525,7 +12477,7 @@
         <v>6</v>
       </c>
       <c r="K150" s="4">
-        <f t="shared" si="92"/>
+        <f t="shared" si="94"/>
         <v>6</v>
       </c>
       <c r="L150" s="4">
@@ -12546,11 +12498,11 @@
         <v>3.5</v>
       </c>
       <c r="D151" s="4">
-        <f t="shared" si="90"/>
+        <f t="shared" si="92"/>
         <v>3</v>
       </c>
       <c r="E151" s="15">
-        <f t="shared" si="95"/>
+        <f t="shared" si="97"/>
         <v>10.5</v>
       </c>
       <c r="F151" s="44"/>
@@ -12564,7 +12516,7 @@
         <v>3</v>
       </c>
       <c r="K151" s="4">
-        <f t="shared" si="92"/>
+        <f t="shared" si="94"/>
         <v>3</v>
       </c>
       <c r="L151" s="4">
@@ -12585,11 +12537,11 @@
         <v>0.39</v>
       </c>
       <c r="D152" s="4">
-        <f t="shared" si="90"/>
+        <f t="shared" si="92"/>
         <v>3</v>
       </c>
       <c r="E152" s="15">
-        <f t="shared" si="95"/>
+        <f t="shared" si="97"/>
         <v>1.17</v>
       </c>
       <c r="F152" s="12">
@@ -12610,7 +12562,7 @@
         <v>3</v>
       </c>
       <c r="K152" s="4">
-        <f t="shared" si="92"/>
+        <f t="shared" si="94"/>
         <v>3</v>
       </c>
       <c r="L152" s="4">
@@ -12631,11 +12583,11 @@
         <v>0.86</v>
       </c>
       <c r="D153" s="4">
-        <f t="shared" si="90"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="E153" s="15">
-        <f t="shared" si="95"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="F153" s="12">
@@ -12656,7 +12608,7 @@
         <v>0</v>
       </c>
       <c r="K153" s="4">
-        <f t="shared" si="92"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="L153" s="4">
@@ -12677,11 +12629,11 @@
         <v>0.11</v>
       </c>
       <c r="D154" s="4">
-        <f t="shared" si="90"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="E154" s="15">
-        <f t="shared" si="95"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="F154" s="12">
@@ -12702,7 +12654,7 @@
         <v>0</v>
       </c>
       <c r="K154" s="4">
-        <f t="shared" si="92"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="L154" s="4">
@@ -12724,11 +12676,11 @@
         <v>1.4E-2</v>
       </c>
       <c r="D155" s="4">
-        <f t="shared" si="90"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="E155" s="15">
-        <f t="shared" ref="E155" si="96">D155*C155</f>
+        <f t="shared" ref="E155" si="98">D155*C155</f>
         <v>0</v>
       </c>
       <c r="F155" s="12">
@@ -12749,7 +12701,7 @@
         <v>0</v>
       </c>
       <c r="K155" s="4">
-        <f t="shared" si="92"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="L155" s="4">
@@ -12762,7 +12714,7 @@
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B156" s="6" t="s">
         <v>36</v>
@@ -12860,97 +12812,97 @@
     <hyperlink ref="B138" r:id="rId34"/>
     <hyperlink ref="B139" r:id="rId35"/>
     <hyperlink ref="B136" r:id="rId36"/>
-    <hyperlink ref="B57" r:id="rId37"/>
-    <hyperlink ref="B153" r:id="rId38"/>
-    <hyperlink ref="B109" r:id="rId39"/>
-    <hyperlink ref="B127" r:id="rId40"/>
-    <hyperlink ref="B114" r:id="rId41"/>
-    <hyperlink ref="B61" r:id="rId42"/>
-    <hyperlink ref="B110" r:id="rId43"/>
-    <hyperlink ref="B119" r:id="rId44"/>
-    <hyperlink ref="B120" r:id="rId45"/>
-    <hyperlink ref="B147" r:id="rId46"/>
-    <hyperlink ref="B149" r:id="rId47"/>
-    <hyperlink ref="B144" r:id="rId48"/>
-    <hyperlink ref="B111" r:id="rId49"/>
-    <hyperlink ref="B145" r:id="rId50"/>
-    <hyperlink ref="B148" r:id="rId51"/>
-    <hyperlink ref="B112" r:id="rId52"/>
-    <hyperlink ref="B87" r:id="rId53"/>
-    <hyperlink ref="B89" r:id="rId54"/>
-    <hyperlink ref="B137" r:id="rId55"/>
-    <hyperlink ref="B38" r:id="rId56"/>
-    <hyperlink ref="B104" r:id="rId57"/>
-    <hyperlink ref="B42" r:id="rId58"/>
-    <hyperlink ref="B43" r:id="rId59"/>
-    <hyperlink ref="B80" r:id="rId60"/>
-    <hyperlink ref="B78" r:id="rId61"/>
-    <hyperlink ref="B81" r:id="rId62"/>
-    <hyperlink ref="B82" r:id="rId63"/>
-    <hyperlink ref="B35" r:id="rId64"/>
-    <hyperlink ref="B32" r:id="rId65"/>
-    <hyperlink ref="B28" r:id="rId66"/>
-    <hyperlink ref="B30" r:id="rId67"/>
-    <hyperlink ref="B31" r:id="rId68"/>
-    <hyperlink ref="B33" r:id="rId69"/>
-    <hyperlink ref="B34" r:id="rId70"/>
-    <hyperlink ref="B62" r:id="rId71"/>
-    <hyperlink ref="B54" r:id="rId72"/>
-    <hyperlink ref="B113" r:id="rId73"/>
-    <hyperlink ref="B108" r:id="rId74"/>
-    <hyperlink ref="B83" r:id="rId75"/>
-    <hyperlink ref="B79" r:id="rId76"/>
-    <hyperlink ref="B67" r:id="rId77"/>
-    <hyperlink ref="B68" r:id="rId78"/>
-    <hyperlink ref="B69" r:id="rId79"/>
-    <hyperlink ref="B44" r:id="rId80"/>
-    <hyperlink ref="B84" r:id="rId81"/>
-    <hyperlink ref="B150" r:id="rId82"/>
-    <hyperlink ref="B146" r:id="rId83"/>
-    <hyperlink ref="B152" r:id="rId84"/>
-    <hyperlink ref="B59" r:id="rId85"/>
-    <hyperlink ref="B60" r:id="rId86"/>
-    <hyperlink ref="B154" r:id="rId87"/>
-    <hyperlink ref="B155" r:id="rId88"/>
-    <hyperlink ref="B121" r:id="rId89"/>
-    <hyperlink ref="B151" r:id="rId90"/>
-    <hyperlink ref="B29" r:id="rId91"/>
-    <hyperlink ref="B70" r:id="rId92"/>
-    <hyperlink ref="B71" r:id="rId93"/>
-    <hyperlink ref="B72" r:id="rId94"/>
-    <hyperlink ref="B73" r:id="rId95"/>
-    <hyperlink ref="B75" r:id="rId96"/>
-    <hyperlink ref="B74" r:id="rId97"/>
-    <hyperlink ref="B3" r:id="rId98"/>
-    <hyperlink ref="B21" r:id="rId99"/>
-    <hyperlink ref="B22" r:id="rId100"/>
-    <hyperlink ref="B23" r:id="rId101"/>
-    <hyperlink ref="B20" r:id="rId102"/>
-    <hyperlink ref="B16" r:id="rId103"/>
-    <hyperlink ref="B24" r:id="rId104"/>
-    <hyperlink ref="B25" r:id="rId105"/>
-    <hyperlink ref="B46" r:id="rId106"/>
-    <hyperlink ref="B47" r:id="rId107"/>
-    <hyperlink ref="B50" r:id="rId108"/>
-    <hyperlink ref="B36" r:id="rId109"/>
-    <hyperlink ref="B39" r:id="rId110"/>
-    <hyperlink ref="B40" r:id="rId111"/>
-    <hyperlink ref="B26" r:id="rId112"/>
-    <hyperlink ref="B6" r:id="rId113"/>
-    <hyperlink ref="B11" r:id="rId114"/>
-    <hyperlink ref="B12" r:id="rId115"/>
-    <hyperlink ref="B13" r:id="rId116"/>
-    <hyperlink ref="B14" r:id="rId117"/>
-    <hyperlink ref="B15" r:id="rId118"/>
-    <hyperlink ref="B56" r:id="rId119"/>
-    <hyperlink ref="B51" r:id="rId120"/>
-    <hyperlink ref="B52" r:id="rId121"/>
-    <hyperlink ref="B10" r:id="rId122" location="93505a472/=1ap2f2s"/>
-    <hyperlink ref="B9" r:id="rId123" location="90760a005/=1ap2f50"/>
-    <hyperlink ref="B8" r:id="rId124" location="90272a105/=1ap2f59"/>
-    <hyperlink ref="B4" r:id="rId125"/>
-    <hyperlink ref="B5" r:id="rId126"/>
-    <hyperlink ref="B48" r:id="rId127"/>
+    <hyperlink ref="B153" r:id="rId37"/>
+    <hyperlink ref="B109" r:id="rId38"/>
+    <hyperlink ref="B127" r:id="rId39"/>
+    <hyperlink ref="B114" r:id="rId40"/>
+    <hyperlink ref="B61" r:id="rId41"/>
+    <hyperlink ref="B110" r:id="rId42"/>
+    <hyperlink ref="B119" r:id="rId43"/>
+    <hyperlink ref="B120" r:id="rId44"/>
+    <hyperlink ref="B147" r:id="rId45"/>
+    <hyperlink ref="B149" r:id="rId46"/>
+    <hyperlink ref="B144" r:id="rId47"/>
+    <hyperlink ref="B111" r:id="rId48"/>
+    <hyperlink ref="B145" r:id="rId49"/>
+    <hyperlink ref="B148" r:id="rId50"/>
+    <hyperlink ref="B112" r:id="rId51"/>
+    <hyperlink ref="B87" r:id="rId52"/>
+    <hyperlink ref="B89" r:id="rId53"/>
+    <hyperlink ref="B137" r:id="rId54"/>
+    <hyperlink ref="B38" r:id="rId55"/>
+    <hyperlink ref="B104" r:id="rId56"/>
+    <hyperlink ref="B42" r:id="rId57"/>
+    <hyperlink ref="B43" r:id="rId58"/>
+    <hyperlink ref="B80" r:id="rId59"/>
+    <hyperlink ref="B78" r:id="rId60"/>
+    <hyperlink ref="B81" r:id="rId61"/>
+    <hyperlink ref="B82" r:id="rId62"/>
+    <hyperlink ref="B35" r:id="rId63"/>
+    <hyperlink ref="B32" r:id="rId64"/>
+    <hyperlink ref="B28" r:id="rId65"/>
+    <hyperlink ref="B30" r:id="rId66"/>
+    <hyperlink ref="B31" r:id="rId67"/>
+    <hyperlink ref="B33" r:id="rId68"/>
+    <hyperlink ref="B34" r:id="rId69"/>
+    <hyperlink ref="B62" r:id="rId70"/>
+    <hyperlink ref="B54" r:id="rId71"/>
+    <hyperlink ref="B113" r:id="rId72"/>
+    <hyperlink ref="B108" r:id="rId73"/>
+    <hyperlink ref="B83" r:id="rId74"/>
+    <hyperlink ref="B79" r:id="rId75"/>
+    <hyperlink ref="B67" r:id="rId76"/>
+    <hyperlink ref="B68" r:id="rId77"/>
+    <hyperlink ref="B69" r:id="rId78"/>
+    <hyperlink ref="B44" r:id="rId79"/>
+    <hyperlink ref="B84" r:id="rId80"/>
+    <hyperlink ref="B150" r:id="rId81"/>
+    <hyperlink ref="B146" r:id="rId82"/>
+    <hyperlink ref="B152" r:id="rId83"/>
+    <hyperlink ref="B59" r:id="rId84"/>
+    <hyperlink ref="B60" r:id="rId85"/>
+    <hyperlink ref="B154" r:id="rId86"/>
+    <hyperlink ref="B155" r:id="rId87"/>
+    <hyperlink ref="B121" r:id="rId88"/>
+    <hyperlink ref="B151" r:id="rId89"/>
+    <hyperlink ref="B29" r:id="rId90"/>
+    <hyperlink ref="B70" r:id="rId91"/>
+    <hyperlink ref="B71" r:id="rId92"/>
+    <hyperlink ref="B72" r:id="rId93"/>
+    <hyperlink ref="B73" r:id="rId94"/>
+    <hyperlink ref="B75" r:id="rId95"/>
+    <hyperlink ref="B74" r:id="rId96"/>
+    <hyperlink ref="B3" r:id="rId97"/>
+    <hyperlink ref="B21" r:id="rId98"/>
+    <hyperlink ref="B22" r:id="rId99"/>
+    <hyperlink ref="B23" r:id="rId100"/>
+    <hyperlink ref="B20" r:id="rId101"/>
+    <hyperlink ref="B16" r:id="rId102"/>
+    <hyperlink ref="B24" r:id="rId103"/>
+    <hyperlink ref="B25" r:id="rId104"/>
+    <hyperlink ref="B46" r:id="rId105"/>
+    <hyperlink ref="B47" r:id="rId106"/>
+    <hyperlink ref="B50" r:id="rId107"/>
+    <hyperlink ref="B36" r:id="rId108"/>
+    <hyperlink ref="B39" r:id="rId109"/>
+    <hyperlink ref="B40" r:id="rId110"/>
+    <hyperlink ref="B26" r:id="rId111"/>
+    <hyperlink ref="B6" r:id="rId112"/>
+    <hyperlink ref="B11" r:id="rId113"/>
+    <hyperlink ref="B12" r:id="rId114"/>
+    <hyperlink ref="B13" r:id="rId115"/>
+    <hyperlink ref="B14" r:id="rId116"/>
+    <hyperlink ref="B15" r:id="rId117"/>
+    <hyperlink ref="B56" r:id="rId118"/>
+    <hyperlink ref="B51" r:id="rId119"/>
+    <hyperlink ref="B52" r:id="rId120"/>
+    <hyperlink ref="B10" r:id="rId121" location="93505a472/=1ap2f2s"/>
+    <hyperlink ref="B9" r:id="rId122" location="90760a005/=1ap2f50"/>
+    <hyperlink ref="B8" r:id="rId123" location="90272a105/=1ap2f59"/>
+    <hyperlink ref="B4" r:id="rId124"/>
+    <hyperlink ref="B5" r:id="rId125"/>
+    <hyperlink ref="B48" r:id="rId126"/>
+    <hyperlink ref="B57" r:id="rId127"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId128"/>
@@ -12959,10 +12911,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12973,29 +12925,33 @@
     <col min="5" max="5" width="12.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="54" t="s">
-        <v>368</v>
+      <c r="C1" s="53" t="s">
+        <v>102</v>
       </c>
       <c r="D1" s="4"/>
-      <c r="E1" s="54" t="s">
-        <v>367</v>
+      <c r="E1" s="53" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="54"/>
+      <c r="C2" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="54" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -13008,17 +12964,17 @@
         <v>14.62</v>
       </c>
       <c r="D3" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E3" s="50">
-        <v>43.86</v>
-      </c>
-      <c r="G3" t="s">
-        <v>369</v>
-      </c>
-      <c r="H3" s="3">
-        <f>SUM(E3)</f>
-        <v>43.86</v>
+        <v>87.72</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="H3" s="50">
+        <f>E3</f>
+        <v>87.72</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -13036,662 +12992,334 @@
         <v>40</v>
       </c>
       <c r="C5" s="5">
-        <v>35.1</v>
+        <v>36.99</v>
       </c>
       <c r="D5" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E5" s="50">
-        <v>105.30000000000001</v>
+        <v>221.94</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>365</v>
+        <v>100</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="5">
-        <v>7.33</v>
+        <v>9.99</v>
       </c>
       <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="50">
-        <v>7.33</v>
+        <v>6</v>
+      </c>
+      <c r="E6" s="5">
+        <v>59.94</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="H6" s="50">
+        <f>SUM(E5:E6)</f>
+        <v>281.88</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>364</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="5">
-        <v>4.6900000000000004</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="50">
-        <v>4.6900000000000004</v>
-      </c>
+      <c r="A7" s="27"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>100</v>
+      <c r="A8" s="19" t="s">
+        <v>360</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C8" s="5">
-        <v>9.99</v>
+        <v>3.26</v>
       </c>
       <c r="D8" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E8" s="50">
-        <v>29.97</v>
+        <v>19.559999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>106</v>
+      <c r="A9" s="19" t="s">
+        <v>348</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C9" s="5">
-        <v>9.99</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D9" s="4">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E9" s="50">
-        <v>19.98</v>
-      </c>
-      <c r="G9" t="s">
-        <v>369</v>
-      </c>
-      <c r="H9" s="3">
-        <f>SUM(E5:E9)</f>
-        <v>167.27</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="30"/>
+      <c r="A10" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>10</v>
+      </c>
+      <c r="E10" s="50">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>362</v>
+      <c r="A11" s="19" t="s">
+        <v>351</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C11" s="5">
-        <v>0.53</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D11" s="4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E11" s="50">
-        <v>6.36</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>366</v>
+      <c r="A12" s="4" t="s">
+        <v>359</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="5">
-        <v>0.13700000000000001</v>
+        <v>2.29</v>
       </c>
       <c r="D12" s="4">
-        <v>50</v>
-      </c>
-      <c r="E12" s="50">
-        <v>6.8500000000000005</v>
+        <v>3</v>
+      </c>
+      <c r="E12" s="5">
+        <v>6.87</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>359</v>
+      <c r="A13" s="4" t="s">
+        <v>372</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="5">
-        <v>2.29</v>
+        <v>3.08</v>
       </c>
       <c r="D13" s="4">
-        <v>3</v>
-      </c>
-      <c r="E13" s="50">
-        <v>6.87</v>
+        <v>10</v>
+      </c>
+      <c r="E13" s="5">
+        <v>30.8</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>336</v>
+        <v>373</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="5">
-        <v>0.41</v>
+        <v>4.28</v>
       </c>
       <c r="D14" s="4">
         <v>10</v>
       </c>
-      <c r="E14" s="50">
-        <v>4.0999999999999996</v>
+      <c r="E14" s="5">
+        <v>42.800000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>333</v>
+        <v>369</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="5">
-        <v>0.42</v>
+        <v>4.57</v>
       </c>
       <c r="D15" s="4">
-        <v>10</v>
-      </c>
-      <c r="E15" s="50">
-        <v>4.2</v>
+        <v>6</v>
+      </c>
+      <c r="E15" s="5">
+        <v>27.42</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>334</v>
+        <v>46</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="5">
-        <v>0.81</v>
+        <v>0.16</v>
       </c>
       <c r="D16" s="4">
         <v>10</v>
       </c>
-      <c r="E16" s="50">
-        <v>8.1000000000000014</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="5">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>335</v>
+        <v>71</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="5">
-        <v>0.42</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="D17" s="4">
         <v>10</v>
       </c>
-      <c r="E17" s="50">
-        <v>4.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>345</v>
+      <c r="E17" s="5">
+        <v>11.100000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="5">
-        <v>1.4999999999999999E-2</v>
+        <v>1.96</v>
       </c>
       <c r="D18" s="4">
         <v>10</v>
       </c>
-      <c r="E18" s="50">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>346</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="5">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="D19" s="4">
-        <v>10</v>
-      </c>
-      <c r="E19" s="50">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>348</v>
+      <c r="E18" s="5">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="H18" s="50">
+        <f>SUM(E8:E18)</f>
+        <v>160.19999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="27"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="28"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>374</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>36</v>
+        <v>375</v>
       </c>
       <c r="C20" s="5">
-        <v>1.4999999999999999E-2</v>
+        <v>0.68</v>
       </c>
       <c r="D20" s="4">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E20" s="50">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>349</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="5">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="D21" s="4">
-        <v>10</v>
-      </c>
-      <c r="E21" s="50">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>350</v>
+        <v>16.32</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="H20" s="50">
+        <f>E20</f>
+        <v>16.32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="27"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="30"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>380</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C22" s="5">
-        <v>1.4999999999999999E-2</v>
+        <v>18.8</v>
       </c>
       <c r="D22" s="4">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E22" s="50">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
-        <v>351</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="5">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="D23" s="4">
-        <v>10</v>
-      </c>
-      <c r="E23" s="50">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
-        <v>352</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="5">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="D24" s="4">
-        <v>10</v>
-      </c>
-      <c r="E24" s="50">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
-        <v>353</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="5">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="D25" s="4">
-        <v>10</v>
-      </c>
-      <c r="E25" s="50">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
-        <v>342</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="5">
-        <v>0.12</v>
-      </c>
-      <c r="D26" s="4">
-        <v>10</v>
-      </c>
-      <c r="E26" s="50">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
-        <v>344</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="D27" s="4">
-        <v>10</v>
-      </c>
-      <c r="E27" s="50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
-        <v>343</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="5">
-        <v>0.48</v>
-      </c>
-      <c r="D28" s="4">
-        <v>10</v>
-      </c>
-      <c r="E28" s="50">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="5">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="D29" s="4">
-        <v>10</v>
-      </c>
-      <c r="E29" s="50">
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="5">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="D30" s="4">
-        <v>10</v>
-      </c>
-      <c r="E30" s="50">
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="5">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="D31" s="4">
-        <v>10</v>
-      </c>
-      <c r="E31" s="50">
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
-        <v>312</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="5">
-        <v>1.03</v>
-      </c>
-      <c r="D32" s="4">
-        <v>10</v>
-      </c>
-      <c r="E32" s="50">
-        <v>10.3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="5">
-        <v>4.57</v>
-      </c>
-      <c r="D33" s="4">
-        <v>3</v>
-      </c>
-      <c r="E33" s="50">
-        <v>13.71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="5">
-        <v>0.16</v>
-      </c>
-      <c r="D34" s="4">
-        <v>10</v>
-      </c>
-      <c r="E34" s="50">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="5">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="D35" s="4">
-        <v>3</v>
-      </c>
-      <c r="E35" s="50">
-        <v>3.33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="5">
-        <v>1.96</v>
-      </c>
-      <c r="D36" s="4">
-        <v>3</v>
-      </c>
-      <c r="E36" s="50">
-        <v>5.88</v>
-      </c>
-      <c r="G36" t="s">
-        <v>369</v>
-      </c>
-      <c r="H36" s="3">
-        <f>SUM(E11:E36)</f>
-        <v>92.399999999999991</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="27"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="30"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>358</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" s="5">
-        <v>28.2</v>
-      </c>
-      <c r="D38" s="4">
-        <v>3</v>
-      </c>
-      <c r="E38" s="50">
-        <v>84.6</v>
-      </c>
-      <c r="G38" t="s">
-        <v>369</v>
-      </c>
-      <c r="H38" s="3">
-        <f>SUM(E38)</f>
-        <v>84.6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
-      <c r="B39" s="29"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="30"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
-        <v>354</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" s="5">
-        <v>8.9499999999999993</v>
-      </c>
-      <c r="D40" s="4">
-        <v>3</v>
-      </c>
-      <c r="E40" s="50">
-        <v>26.849999999999998</v>
-      </c>
-      <c r="G40" t="s">
-        <v>369</v>
-      </c>
-      <c r="H40" s="3">
-        <f>SUM(E40)</f>
-        <v>26.849999999999998</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D42" s="4" t="s">
+        <v>112.8</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="H22" s="50">
+        <f>E22</f>
+        <v>112.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D24" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E42" s="5">
-        <f>SUM(E3:E40)</f>
-        <v>414.98</v>
+      <c r="E24" s="5">
+        <f>SUM(E3:E22)</f>
+        <v>658.92</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E40">
-    <sortState ref="A3:E62">
-      <sortCondition ref="B2:B62"/>
+  <autoFilter ref="A2:E22">
+    <sortState ref="A3:E18">
+      <sortCondition ref="B2:B18"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="2">
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="C1:C2"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B32" r:id="rId1"/>
-    <hyperlink ref="B34" r:id="rId2"/>
-    <hyperlink ref="B35" r:id="rId3"/>
-    <hyperlink ref="B26" r:id="rId4"/>
-    <hyperlink ref="B29" r:id="rId5"/>
-    <hyperlink ref="B30" r:id="rId6"/>
-    <hyperlink ref="B24" r:id="rId7"/>
-    <hyperlink ref="B21" r:id="rId8"/>
-    <hyperlink ref="B18" r:id="rId9"/>
-    <hyperlink ref="B20" r:id="rId10"/>
-    <hyperlink ref="B22" r:id="rId11"/>
-    <hyperlink ref="B23" r:id="rId12"/>
-    <hyperlink ref="B36" r:id="rId13"/>
-    <hyperlink ref="B8" r:id="rId14"/>
-    <hyperlink ref="B9" r:id="rId15"/>
-    <hyperlink ref="B31" r:id="rId16"/>
-    <hyperlink ref="B19" r:id="rId17"/>
-    <hyperlink ref="B38" r:id="rId18"/>
-    <hyperlink ref="B15" r:id="rId19"/>
-    <hyperlink ref="B16" r:id="rId20"/>
-    <hyperlink ref="B17" r:id="rId21"/>
-    <hyperlink ref="B14" r:id="rId22"/>
-    <hyperlink ref="B3" r:id="rId23"/>
-    <hyperlink ref="B40" r:id="rId24"/>
-    <hyperlink ref="B25" r:id="rId25"/>
-    <hyperlink ref="B27" r:id="rId26"/>
-    <hyperlink ref="B28" r:id="rId27"/>
-    <hyperlink ref="B13" r:id="rId28"/>
-    <hyperlink ref="B5" r:id="rId29"/>
-    <hyperlink ref="B11" r:id="rId30"/>
-    <hyperlink ref="B6" r:id="rId31"/>
-    <hyperlink ref="B7" r:id="rId32"/>
-    <hyperlink ref="B12" r:id="rId33"/>
-    <hyperlink ref="B33" r:id="rId34"/>
+    <hyperlink ref="B16" r:id="rId1"/>
+    <hyperlink ref="B17" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId3"/>
+    <hyperlink ref="B10" r:id="rId4"/>
+    <hyperlink ref="B11" r:id="rId5"/>
+    <hyperlink ref="B18" r:id="rId6"/>
+    <hyperlink ref="B6" r:id="rId7"/>
+    <hyperlink ref="B3" r:id="rId8"/>
+    <hyperlink ref="B8" r:id="rId9"/>
+    <hyperlink ref="B5" r:id="rId10"/>
+    <hyperlink ref="B15" r:id="rId11"/>
+    <hyperlink ref="B13" r:id="rId12"/>
+    <hyperlink ref="B14" r:id="rId13"/>
+    <hyperlink ref="B20" r:id="rId14" location="93505a472/=1ap2f2s"/>
+    <hyperlink ref="B22" r:id="rId15"/>
+    <hyperlink ref="B12" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14027,22 +13655,22 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="H3" s="55" t="s">
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="H3" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B4" t="s">

</xml_diff>